<commit_message>
Send Bulk emails with tracker
</commit_message>
<xml_diff>
--- a/SendBulkEmails_WithTracker/Data/MailDataAndConfigSheet.xlsx
+++ b/SendBulkEmails_WithTracker/Data/MailDataAndConfigSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\ValueMomentum\POC\HR\TAG_SendBulkEmails\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Uipath\SendBulkEmails_WithTracker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D53F0B-B417-4333-A296-29A3F392C750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2B5FE1-C594-4FF7-B7A2-D334B166E407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-110" windowWidth="18470" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>EmailStatus</t>
   </si>
   <si>
-    <t>vajrang@outlook.com</t>
-  </si>
-  <si>
     <t>Vajrang</t>
   </si>
   <si>
@@ -69,18 +66,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>vajrang@gmail.com</t>
-  </si>
-  <si>
     <t>vajrang19</t>
   </si>
   <si>
     <t>RejectedTemplate</t>
   </si>
   <si>
-    <t>vajrang@yahoo.com</t>
-  </si>
-  <si>
     <t>vajrang1</t>
   </si>
   <si>
@@ -112,6 +103,15 @@
   </si>
   <si>
     <t>hai #applicantname#  You profile is on Hold</t>
+  </si>
+  <si>
+    <t>abc@outlook.com</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>abc@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -442,20 +442,20 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,15 +475,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>VLOOKUP(C2,Templates!A:B,2,FALSE)</f>
@@ -494,21 +494,21 @@
         <v>Hi Vajrang You are shortlisted</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>VLOOKUP(C3,Templates!A:B,2,FALSE)</f>
@@ -519,21 +519,21 @@
         <v>Hello vajrang19  you are rejected</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>VLOOKUP(C4,Templates!A:B,2,FALSE)</f>
@@ -544,17 +544,17 @@
         <v>hai vajrang1  You profile is on Hold</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="vajrang@outlook.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="vajrang@gmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" display="vajrang@yahoo.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -577,57 +577,57 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="17.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.90625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>